<commit_message>
Exported genes associated with diseases
In Excel files containing the most pertinent data from this study, DEGs have been linked to multiple diseases.
</commit_message>
<xml_diff>
--- a/5_Integración con datos de patógenos y enfermedades/Fusobacterium Nucleatum/Valor Padj menor a 0.05/genes_rare_diseases.xlsx
+++ b/5_Integración con datos de patógenos y enfermedades/Fusobacterium Nucleatum/Valor Padj menor a 0.05/genes_rare_diseases.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -640,12 +640,36 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>SNCG</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Autosomal dominant Charcot-Marie-Tooth disease type 2L ORPHA:99945</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>THBS1</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>Familial primary localized cutaneous amyloidosis ORPHA:353220</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TIMP2</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Charcot-Marie-Tooth disease type 1A ORPHA:101081, Charcot-Marie-Tooth disease type 1E ORPHA:90658</t>
         </is>
       </c>
     </row>

</xml_diff>